<commit_message>
swap bleed resistor for SMD
</commit_message>
<xml_diff>
--- a/BOM-nixieAccurateClock.xlsx
+++ b/BOM-nixieAccurateClock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7175D27D-244A-4589-A467-8792F1106101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4AFFD-7FAB-4C6E-90E0-0756BD50682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,12 +463,6 @@
     <t>https://www.vishay.com/docs/30122/wslp.pdf</t>
   </si>
   <si>
-    <t>Resistor_THT:R_Axial_DIN0617_L17.0mm_D6.0mm_P20.32mm_Horizontal</t>
-  </si>
-  <si>
-    <t>https://www.te.com/usa-en/product-8-2176412-0.datasheet.pdf</t>
-  </si>
-  <si>
     <t>Device:R_Potentiometer</t>
   </si>
   <si>
@@ -619,9 +613,6 @@
     <t>RMCF0603FT1M00</t>
   </si>
   <si>
-    <t>ROX5SSJ10K</t>
-  </si>
-  <si>
     <t>3266Z-1-104LF</t>
   </si>
   <si>
@@ -826,12 +817,6 @@
     <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT1M00/1761036</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/ROX5SSJ10K?qs=gZXFycFWdAPK2TCKEiyMYg%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/ROX5SSJ10K/9926250</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/bourns-inc/3266Z-1-104LF/3722105</t>
   </si>
   <si>
@@ -878,6 +863,21 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/Texas-Instruments/TXB0108PWR?qs=oFXvjAmG9EgEUWGWzOVFCA%3D%3D</t>
+  </si>
+  <si>
+    <t>352010KJT</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_2512_6332Metric</t>
+  </si>
+  <si>
+    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=1773139&amp;DocType=DS&amp;DocLang=English</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-passive-product/352010KJT/2364839</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/352010KJT?qs=DDevMFOh4ssnVH2d0oCe7g%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA59D120-68A1-4021-9F61-63CF243C8D9C}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1267,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1342,10 +1342,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1381,10 +1381,10 @@
         <v>113</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1395,7 +1395,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1420,10 +1420,10 @@
         <v>21</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1440,7 +1440,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1459,10 +1459,10 @@
         <v>116</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1479,7 +1479,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G13" s="1">
         <v>1.03</v>
@@ -1498,10 +1498,10 @@
         <v>119</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1518,7 +1518,7 @@
         <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -1537,10 +1537,10 @@
         <v>120</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1573,10 +1573,10 @@
         <v>123</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1587,13 +1587,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -1612,10 +1612,10 @@
         <v>126</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1651,10 +1651,10 @@
         <v>129</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1671,7 +1671,7 @@
         <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G18" s="1">
         <v>0.81</v>
@@ -1690,10 +1690,10 @@
         <v>131</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="M18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1710,7 +1710,7 @@
         <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G19" s="1">
         <v>0.38</v>
@@ -1729,10 +1729,10 @@
         <v>134</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1749,7 +1749,7 @@
         <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G20" s="1">
         <v>4.07</v>
@@ -1768,10 +1768,10 @@
         <v>136</v>
       </c>
       <c r="L20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1807,10 +1807,10 @@
         <v>139</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1827,7 +1827,7 @@
         <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
@@ -1846,10 +1846,10 @@
         <v>37</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1866,7 +1866,7 @@
         <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -1885,10 +1885,10 @@
         <v>141</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1905,7 +1905,7 @@
         <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G24" s="1">
         <v>0.1</v>
@@ -1924,10 +1924,10 @@
         <v>37</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1944,7 +1944,7 @@
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G25" s="1">
         <v>0.74</v>
@@ -1963,10 +1963,10 @@
         <v>142</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1983,7 +1983,7 @@
         <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G26" s="1">
         <v>0.1</v>
@@ -2002,10 +2002,10 @@
         <v>37</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2022,7 +2022,7 @@
         <v>470</v>
       </c>
       <c r="E27" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G27" s="1">
         <v>0.1</v>
@@ -2041,10 +2041,10 @@
         <v>37</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2061,7 +2061,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G28" s="1">
         <v>0.1</v>
@@ -2080,10 +2080,10 @@
         <v>141</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2100,7 +2100,7 @@
         <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G29" s="1">
         <v>0.1</v>
@@ -2119,10 +2119,10 @@
         <v>37</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2139,7 +2139,7 @@
         <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G30" s="1">
         <v>0.1</v>
@@ -2158,10 +2158,10 @@
         <v>141</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2178,7 +2178,7 @@
         <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G31" s="1">
         <v>0.1</v>
@@ -2197,10 +2197,10 @@
         <v>37</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2217,7 +2217,7 @@
         <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G32" s="1">
         <v>0.1</v>
@@ -2236,10 +2236,10 @@
         <v>37</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2256,7 +2256,7 @@
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G33" s="1">
         <v>0.1</v>
@@ -2275,10 +2275,10 @@
         <v>37</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2295,7 +2295,7 @@
         <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G34" s="1">
         <v>0.1</v>
@@ -2314,10 +2314,10 @@
         <v>141</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2334,29 +2334,29 @@
         <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>195</v>
+        <v>277</v>
       </c>
       <c r="G35" s="1">
-        <v>0.6</v>
+        <v>0.43</v>
       </c>
       <c r="H35" s="1">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.43</v>
       </c>
       <c r="I35" t="s">
         <v>35</v>
       </c>
       <c r="J35" t="s">
-        <v>143</v>
+        <v>278</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>144</v>
+        <v>279</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2373,7 +2373,7 @@
         <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G36" s="1">
         <v>2.13</v>
@@ -2383,19 +2383,19 @@
         <v>2.13</v>
       </c>
       <c r="I36" t="s">
+        <v>143</v>
+      </c>
+      <c r="J36" t="s">
+        <v>144</v>
+      </c>
+      <c r="K36" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J36" t="s">
-        <v>146</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="L36" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2412,7 +2412,7 @@
         <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G37" s="1">
         <v>1.75</v>
@@ -2422,19 +2422,19 @@
         <v>1.75</v>
       </c>
       <c r="I37" t="s">
+        <v>146</v>
+      </c>
+      <c r="J37" t="s">
+        <v>147</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="J37" t="s">
-        <v>149</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="L37" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2461,19 +2461,19 @@
         <v>7.6</v>
       </c>
       <c r="I38" t="s">
+        <v>149</v>
+      </c>
+      <c r="J38" t="s">
+        <v>150</v>
+      </c>
+      <c r="K38" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="J38" t="s">
-        <v>152</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>153</v>
-      </c>
       <c r="L38" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2490,7 +2490,7 @@
         <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="G39" s="1">
         <v>1.37</v>
@@ -2500,19 +2500,19 @@
         <v>1.37</v>
       </c>
       <c r="I39" t="s">
+        <v>152</v>
+      </c>
+      <c r="J39" t="s">
+        <v>153</v>
+      </c>
+      <c r="K39" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="J39" t="s">
-        <v>155</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="L39" s="3" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2536,19 +2536,19 @@
         <v>35</v>
       </c>
       <c r="I40" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L40" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M40" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2572,19 +2572,19 @@
         <v>0.97</v>
       </c>
       <c r="I41" t="s">
+        <v>157</v>
+      </c>
+      <c r="J41" t="s">
+        <v>158</v>
+      </c>
+      <c r="K41" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="J41" t="s">
-        <v>160</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>161</v>
-      </c>
       <c r="L41" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2608,19 +2608,19 @@
         <v>27.8</v>
       </c>
       <c r="I42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M42" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2634,7 +2634,7 @@
         <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E43" t="s">
         <v>107</v>
@@ -2647,19 +2647,19 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="I43" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43" t="s">
+        <v>163</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="J43" t="s">
-        <v>165</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>166</v>
-      </c>
       <c r="L43" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2670,7 +2670,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G44" s="1">
         <f>'IN-14 daughter board'!H15</f>
@@ -2681,16 +2681,16 @@
         <v>127.80000000000003</v>
       </c>
       <c r="I44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="L44" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M44" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2707,7 +2707,7 @@
         <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G45" s="1">
         <v>5.93</v>
@@ -2717,19 +2717,19 @@
         <v>5.93</v>
       </c>
       <c r="I45" t="s">
+        <v>167</v>
+      </c>
+      <c r="J45" t="s">
+        <v>168</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="J45" t="s">
-        <v>170</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="L45" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2740,10 +2740,10 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D46" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E46" t="s">
         <v>110</v>
@@ -2756,25 +2756,25 @@
         <v>3.3</v>
       </c>
       <c r="I46" t="s">
+        <v>170</v>
+      </c>
+      <c r="J46" t="s">
+        <v>171</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="J46" t="s">
-        <v>173</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="L46" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H47" s="1">
         <f>SUM(H10:H46)</f>
-        <v>245.14000000000004</v>
+        <v>244.97000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2983,10 +2983,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="M9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3022,10 +3022,10 @@
         <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3058,10 +3058,10 @@
         <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3094,10 +3094,10 @@
         <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="M12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3133,10 +3133,10 @@
         <v>37</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3169,10 +3169,10 @@
         <v>43</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Switch to SMT test points
</commit_message>
<xml_diff>
--- a/BOM-nixieAccurateClock.xlsx
+++ b/BOM-nixieAccurateClock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB4AFFD-7FAB-4C6E-90E0-0756BD50682A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEE7D8D-E522-4885-81F8-181FFD9EBB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -484,12 +484,6 @@
     <t>Connector:TestPoint</t>
   </si>
   <si>
-    <t>TestPoint:TestPoint_Loop_D2.54mm_Drill1.5mm_Beaded</t>
-  </si>
-  <si>
-    <t>https://www.keyelco.com/userAssets/file/M65p56.pdf</t>
-  </si>
-  <si>
     <t>Interface_Expansion:MCP23008-xSO</t>
   </si>
   <si>
@@ -829,12 +823,6 @@
     <t>https://www.mouser.com/ProductDetail/TE-Connectivity-PB/ADE0804?qs=k5V78Jg%2Feq6GvBeNB1YtWA%3D%3D</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/keystone-electronics/5001/255327</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/Keystone-Electronics/5001?qs=q0tsjPZWdm%2FW0vdr%2FwowKg%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Microchip-Technology/MCP23008-E-SO?qs=Sez7gRs8XSWum74ZwQXTLw%3D%3D</t>
   </si>
   <si>
@@ -878,6 +866,18 @@
   </si>
   <si>
     <t>https://www.mouser.com/ProductDetail/TE-Connectivity-Holsworthy/352010KJT?qs=DDevMFOh4ssnVH2d0oCe7g%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/keystone-electronics/5019/3907343</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Keystone-Electronics/5019?qs=wOxb8XianXjjCAsb90Ilzw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/215/019-743690.pdf</t>
+  </si>
+  <si>
+    <t>00_lib:TestPoint_Keystone_5019_Minature</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA59D120-68A1-4021-9F61-63CF243C8D9C}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F28" zoomScale="136" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1267,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1342,10 +1344,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1381,10 +1383,10 @@
         <v>113</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1395,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1420,10 +1422,10 @@
         <v>21</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1440,7 +1442,7 @@
         <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1459,10 +1461,10 @@
         <v>116</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1479,7 +1481,7 @@
         <v>52</v>
       </c>
       <c r="E13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G13" s="1">
         <v>1.03</v>
@@ -1498,10 +1500,10 @@
         <v>119</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1518,7 +1520,7 @@
         <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -1537,10 +1539,10 @@
         <v>120</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1573,10 +1575,10 @@
         <v>123</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1587,13 +1589,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -1612,10 +1614,10 @@
         <v>126</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1651,10 +1653,10 @@
         <v>129</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1671,7 +1673,7 @@
         <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G18" s="1">
         <v>0.81</v>
@@ -1690,10 +1692,10 @@
         <v>131</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1710,7 +1712,7 @@
         <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G19" s="1">
         <v>0.38</v>
@@ -1729,10 +1731,10 @@
         <v>134</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1749,7 +1751,7 @@
         <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G20" s="1">
         <v>4.07</v>
@@ -1768,10 +1770,10 @@
         <v>136</v>
       </c>
       <c r="L20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1807,10 +1809,10 @@
         <v>139</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1827,7 +1829,7 @@
         <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
@@ -1846,10 +1848,10 @@
         <v>37</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1866,7 +1868,7 @@
         <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -1885,10 +1887,10 @@
         <v>141</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1905,7 +1907,7 @@
         <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G24" s="1">
         <v>0.1</v>
@@ -1924,10 +1926,10 @@
         <v>37</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1944,7 +1946,7 @@
         <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G25" s="1">
         <v>0.74</v>
@@ -1963,10 +1965,10 @@
         <v>142</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -1983,7 +1985,7 @@
         <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G26" s="1">
         <v>0.1</v>
@@ -2002,10 +2004,10 @@
         <v>37</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2022,7 +2024,7 @@
         <v>470</v>
       </c>
       <c r="E27" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G27" s="1">
         <v>0.1</v>
@@ -2041,10 +2043,10 @@
         <v>37</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2061,7 +2063,7 @@
         <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G28" s="1">
         <v>0.1</v>
@@ -2080,10 +2082,10 @@
         <v>141</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2100,7 +2102,7 @@
         <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G29" s="1">
         <v>0.1</v>
@@ -2119,10 +2121,10 @@
         <v>37</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2139,7 +2141,7 @@
         <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G30" s="1">
         <v>0.1</v>
@@ -2158,10 +2160,10 @@
         <v>141</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2178,7 +2180,7 @@
         <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G31" s="1">
         <v>0.1</v>
@@ -2197,10 +2199,10 @@
         <v>37</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2217,7 +2219,7 @@
         <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G32" s="1">
         <v>0.1</v>
@@ -2236,10 +2238,10 @@
         <v>37</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2256,7 +2258,7 @@
         <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G33" s="1">
         <v>0.1</v>
@@ -2275,10 +2277,10 @@
         <v>37</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2295,7 +2297,7 @@
         <v>92</v>
       </c>
       <c r="E34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G34" s="1">
         <v>0.1</v>
@@ -2314,10 +2316,10 @@
         <v>141</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2334,7 +2336,7 @@
         <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="G35" s="1">
         <v>0.43</v>
@@ -2347,16 +2349,16 @@
         <v>35</v>
       </c>
       <c r="J35" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2373,7 +2375,7 @@
         <v>77</v>
       </c>
       <c r="E36" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G36" s="1">
         <v>2.13</v>
@@ -2392,10 +2394,10 @@
         <v>145</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2412,7 +2414,7 @@
         <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G37" s="1">
         <v>1.75</v>
@@ -2431,10 +2433,10 @@
         <v>148</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2451,29 +2453,29 @@
         <v>98</v>
       </c>
       <c r="E38">
-        <v>5001</v>
+        <v>5019</v>
       </c>
       <c r="G38" s="1">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="H38" s="1">
         <f t="shared" si="0"/>
-        <v>7.6</v>
+        <v>6.6000000000000005</v>
       </c>
       <c r="I38" t="s">
         <v>149</v>
       </c>
       <c r="J38" t="s">
-        <v>150</v>
+        <v>281</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>151</v>
+        <v>280</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>265</v>
+        <v>278</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2490,7 +2492,7 @@
         <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G39" s="1">
         <v>1.37</v>
@@ -2500,19 +2502,19 @@
         <v>1.37</v>
       </c>
       <c r="I39" t="s">
+        <v>150</v>
+      </c>
+      <c r="J39" t="s">
+        <v>151</v>
+      </c>
+      <c r="K39" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="J39" t="s">
-        <v>153</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="L39" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2536,19 +2538,19 @@
         <v>35</v>
       </c>
       <c r="I40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="L40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2572,19 +2574,19 @@
         <v>0.97</v>
       </c>
       <c r="I41" t="s">
+        <v>155</v>
+      </c>
+      <c r="J41" t="s">
+        <v>156</v>
+      </c>
+      <c r="K41" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="J41" t="s">
-        <v>158</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>159</v>
-      </c>
       <c r="L41" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2608,19 +2610,19 @@
         <v>27.8</v>
       </c>
       <c r="I42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J42" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2634,7 +2636,7 @@
         <v>106</v>
       </c>
       <c r="D43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E43" t="s">
         <v>107</v>
@@ -2647,19 +2649,19 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="I43" t="s">
+        <v>160</v>
+      </c>
+      <c r="J43" t="s">
+        <v>161</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="J43" t="s">
-        <v>163</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="L43" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2670,7 +2672,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G44" s="1">
         <f>'IN-14 daughter board'!H15</f>
@@ -2681,16 +2683,16 @@
         <v>127.80000000000003</v>
       </c>
       <c r="I44" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2707,7 +2709,7 @@
         <v>109</v>
       </c>
       <c r="E45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G45" s="1">
         <v>5.93</v>
@@ -2717,19 +2719,19 @@
         <v>5.93</v>
       </c>
       <c r="I45" t="s">
+        <v>165</v>
+      </c>
+      <c r="J45" t="s">
+        <v>166</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="J45" t="s">
-        <v>168</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="L45" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2740,10 +2742,10 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D46" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E46" t="s">
         <v>110</v>
@@ -2756,25 +2758,25 @@
         <v>3.3</v>
       </c>
       <c r="I46" t="s">
+        <v>168</v>
+      </c>
+      <c r="J46" t="s">
+        <v>169</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="J46" t="s">
-        <v>171</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>172</v>
-      </c>
       <c r="L46" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="H47" s="1">
         <f>SUM(H10:H46)</f>
-        <v>244.97000000000003</v>
+        <v>243.97000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2983,10 +2985,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3022,10 +3024,10 @@
         <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3058,10 +3060,10 @@
         <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="M11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3094,10 +3096,10 @@
         <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="M12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3133,10 +3135,10 @@
         <v>37</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3169,10 +3171,10 @@
         <v>43</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
switch to 27k R_anode
Add voltage rail jumpers for different 5V and 3.3V standby applications
</commit_message>
<xml_diff>
--- a/BOM-nixieAccurateClock.xlsx
+++ b/BOM-nixieAccurateClock.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEE7D8D-E522-4885-81F8-181FFD9EBB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA6176E-D5BF-432E-9819-DA187A99C34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nixie Accurate Clock" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="281">
   <si>
     <t>Price</t>
   </si>
@@ -136,9 +136,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>33k</t>
-  </si>
-  <si>
     <t>Device:R</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>https://www.yageo.com/upload/media/product/app/datasheet/rchip/pyu-rc_group_51_rohs_l.pdf</t>
   </si>
   <si>
-    <t>RC1206JR-0733KL</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -652,12 +646,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/YAGEO/RC1206JR-0733KL?qs=4sq2y2bXwtTBbhYRyjZ6aQ%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/yageo/RC1206JR-0733KL/729282</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/microchip-technology/HV509K6-G/4902492</t>
   </si>
   <si>
@@ -878,6 +866,15 @@
   </si>
   <si>
     <t>00_lib:TestPoint_Keystone_5019_Minature</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/YAGEO/RC1206JR-0727KL?qs=CteSnpDdeuBg3%2FC0aG6GFQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RC1206JR-0727KL/729262</t>
+  </si>
+  <si>
+    <t>RC1206JR-0727KL</t>
   </si>
 </sst>
 </file>
@@ -949,9 +946,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -989,7 +986,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1095,7 +1092,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1237,7 +1234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1247,32 +1244,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA59D120-68A1-4021-9F61-63CF243C8D9C}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScale="136" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="89.68359375" customWidth="1"/>
-    <col min="4" max="4" width="15.20703125" customWidth="1"/>
-    <col min="5" max="5" width="17.68359375" customWidth="1"/>
-    <col min="9" max="9" width="35.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84.47265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.1015625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1280,7 +1275,7 @@
         <v>45304.804212962961</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1288,7 +1283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1296,7 +1291,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1304,12 +1299,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1317,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -1332,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
@@ -1344,13 +1339,13 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1358,10 +1353,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10">
         <v>103</v>
@@ -1374,22 +1369,22 @@
         <v>1.22</v>
       </c>
       <c r="I10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="J10" t="s">
-        <v>112</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1397,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1413,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J11" t="s">
         <v>20</v>
@@ -1422,13 +1417,13 @@
         <v>21</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -1436,13 +1431,13 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1452,22 +1447,22 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="I12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
         <v>20</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1475,13 +1470,13 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" s="1">
         <v>1.03</v>
@@ -1491,22 +1486,22 @@
         <v>2.06</v>
       </c>
       <c r="I13" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J13" t="s">
-        <v>118</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1514,13 +1509,13 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -1530,22 +1525,22 @@
         <v>0.1</v>
       </c>
       <c r="I14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1553,10 +1548,10 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1">
         <v>0.27</v>
@@ -1566,22 +1561,22 @@
         <v>0.81</v>
       </c>
       <c r="I15" t="s">
+        <v>119</v>
+      </c>
+      <c r="J15" t="s">
+        <v>120</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="J15" t="s">
-        <v>122</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="L15" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1589,13 +1584,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -1605,22 +1600,22 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="I16" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" t="s">
+        <v>123</v>
+      </c>
+      <c r="K16" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="J16" t="s">
-        <v>125</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="L16" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>8</v>
       </c>
@@ -1628,10 +1623,10 @@
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17">
         <v>132289</v>
@@ -1644,22 +1639,22 @@
         <v>7.55</v>
       </c>
       <c r="I17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="J17" t="s">
-        <v>128</v>
-      </c>
-      <c r="K17" s="3" t="s">
-        <v>129</v>
-      </c>
       <c r="L17" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>9</v>
       </c>
@@ -1667,13 +1662,13 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G18" s="1">
         <v>0.81</v>
@@ -1686,19 +1681,19 @@
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="M18" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>10</v>
       </c>
@@ -1706,13 +1701,13 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G19" s="1">
         <v>0.38</v>
@@ -1722,22 +1717,22 @@
         <v>0.38</v>
       </c>
       <c r="I19" t="s">
+        <v>130</v>
+      </c>
+      <c r="J19" t="s">
+        <v>131</v>
+      </c>
+      <c r="K19" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="J19" t="s">
-        <v>133</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="L19" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>11</v>
       </c>
@@ -1745,13 +1740,13 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G20" s="1">
         <v>4.07</v>
@@ -1761,22 +1756,22 @@
         <v>4.07</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -1784,13 +1779,13 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G21" s="1">
         <v>0.55000000000000004</v>
@@ -1800,22 +1795,22 @@
         <v>2.75</v>
       </c>
       <c r="I21" t="s">
+        <v>135</v>
+      </c>
+      <c r="J21" t="s">
+        <v>136</v>
+      </c>
+      <c r="K21" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="J21" t="s">
-        <v>138</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="L21" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>13</v>
       </c>
@@ -1823,13 +1818,13 @@
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
@@ -1839,22 +1834,22 @@
         <v>0.4</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>14</v>
       </c>
@@ -1862,13 +1857,13 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -1878,22 +1873,22 @@
         <v>0.2</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>15</v>
       </c>
@@ -1901,13 +1896,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G24" s="1">
         <v>0.1</v>
@@ -1917,22 +1912,22 @@
         <v>0.1</v>
       </c>
       <c r="I24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>16</v>
       </c>
@@ -1940,13 +1935,13 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G25" s="1">
         <v>0.74</v>
@@ -1956,22 +1951,22 @@
         <v>1.48</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J25" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="L25" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>17</v>
       </c>
@@ -1979,13 +1974,13 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G26" s="1">
         <v>0.1</v>
@@ -1995,22 +1990,22 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>18</v>
       </c>
@@ -2018,13 +2013,13 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D27">
         <v>470</v>
       </c>
       <c r="E27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G27" s="1">
         <v>0.1</v>
@@ -2034,22 +2029,22 @@
         <v>0.1</v>
       </c>
       <c r="I27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>19</v>
       </c>
@@ -2057,13 +2052,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G28" s="1">
         <v>0.1</v>
@@ -2073,22 +2068,22 @@
         <v>0.2</v>
       </c>
       <c r="I28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20</v>
       </c>
@@ -2096,13 +2091,13 @@
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G29" s="1">
         <v>0.1</v>
@@ -2112,22 +2107,22 @@
         <v>0.2</v>
       </c>
       <c r="I29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>21</v>
       </c>
@@ -2135,13 +2130,13 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G30" s="1">
         <v>0.1</v>
@@ -2151,22 +2146,22 @@
         <v>0.1</v>
       </c>
       <c r="I30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J30" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>22</v>
       </c>
@@ -2174,13 +2169,13 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G31" s="1">
         <v>0.1</v>
@@ -2190,22 +2185,22 @@
         <v>0.1</v>
       </c>
       <c r="I31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>23</v>
       </c>
@@ -2213,13 +2208,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G32" s="1">
         <v>0.1</v>
@@ -2229,22 +2224,22 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="I32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>24</v>
       </c>
@@ -2252,13 +2247,13 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G33" s="1">
         <v>0.1</v>
@@ -2268,22 +2263,22 @@
         <v>0.1</v>
       </c>
       <c r="I33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>25</v>
       </c>
@@ -2291,13 +2286,13 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E34" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G34" s="1">
         <v>0.1</v>
@@ -2307,22 +2302,22 @@
         <v>0.1</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>26</v>
       </c>
@@ -2330,13 +2325,13 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G35" s="1">
         <v>0.43</v>
@@ -2346,22 +2341,22 @@
         <v>0.43</v>
       </c>
       <c r="I35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J35" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>27</v>
       </c>
@@ -2369,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G36" s="1">
         <v>2.13</v>
@@ -2385,22 +2380,22 @@
         <v>2.13</v>
       </c>
       <c r="I36" t="s">
+        <v>141</v>
+      </c>
+      <c r="J36" t="s">
+        <v>142</v>
+      </c>
+      <c r="K36" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="J36" t="s">
-        <v>144</v>
-      </c>
-      <c r="K36" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="L36" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>28</v>
       </c>
@@ -2408,13 +2403,13 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E37" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G37" s="1">
         <v>1.75</v>
@@ -2424,22 +2419,22 @@
         <v>1.75</v>
       </c>
       <c r="I37" t="s">
+        <v>144</v>
+      </c>
+      <c r="J37" t="s">
+        <v>145</v>
+      </c>
+      <c r="K37" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="J37" t="s">
-        <v>147</v>
-      </c>
-      <c r="K37" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="L37" s="3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>29</v>
       </c>
@@ -2447,10 +2442,10 @@
         <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E38">
         <v>5019</v>
@@ -2463,22 +2458,22 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="I38" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J38" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>30</v>
       </c>
@@ -2486,13 +2481,13 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G39" s="1">
         <v>1.37</v>
@@ -2502,22 +2497,22 @@
         <v>1.37</v>
       </c>
       <c r="I39" t="s">
+        <v>148</v>
+      </c>
+      <c r="J39" t="s">
+        <v>149</v>
+      </c>
+      <c r="K39" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="J39" t="s">
-        <v>151</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="L39" s="3" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>31</v>
       </c>
@@ -2525,10 +2520,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G40" s="1">
         <v>35</v>
@@ -2538,22 +2533,22 @@
         <v>35</v>
       </c>
       <c r="I40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="L40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M40" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>32</v>
       </c>
@@ -2561,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G41" s="1">
         <v>0.97</v>
@@ -2574,22 +2569,22 @@
         <v>0.97</v>
       </c>
       <c r="I41" t="s">
+        <v>153</v>
+      </c>
+      <c r="J41" t="s">
+        <v>154</v>
+      </c>
+      <c r="K41" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="J41" t="s">
-        <v>156</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="L41" s="3" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>33</v>
       </c>
@@ -2597,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G42" s="1">
         <v>27.8</v>
@@ -2610,22 +2605,22 @@
         <v>27.8</v>
       </c>
       <c r="I42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J42" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L42" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M42" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>34</v>
       </c>
@@ -2633,13 +2628,13 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G43" s="1">
         <v>2.1800000000000002</v>
@@ -2649,22 +2644,22 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="I43" t="s">
+        <v>158</v>
+      </c>
+      <c r="J43" t="s">
+        <v>159</v>
+      </c>
+      <c r="K43" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="J43" t="s">
-        <v>161</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="L43" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>35</v>
       </c>
@@ -2672,7 +2667,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G44" s="1">
         <f>'IN-14 daughter board'!H15</f>
@@ -2683,19 +2678,19 @@
         <v>127.80000000000003</v>
       </c>
       <c r="I44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="L44" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M44" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>36</v>
       </c>
@@ -2703,13 +2698,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G45" s="1">
         <v>5.93</v>
@@ -2719,22 +2714,22 @@
         <v>5.93</v>
       </c>
       <c r="I45" t="s">
+        <v>163</v>
+      </c>
+      <c r="J45" t="s">
+        <v>164</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="J45" t="s">
-        <v>166</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>167</v>
-      </c>
       <c r="L45" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>37</v>
       </c>
@@ -2742,13 +2737,13 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D46" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G46" s="1">
         <v>1.65</v>
@@ -2758,22 +2753,22 @@
         <v>3.3</v>
       </c>
       <c r="I46" t="s">
+        <v>166</v>
+      </c>
+      <c r="J46" t="s">
+        <v>167</v>
+      </c>
+      <c r="K46" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="J46" t="s">
-        <v>169</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="L46" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H47" s="1">
         <f>SUM(H10:H46)</f>
         <v>243.97000000000003</v>
@@ -2894,26 +2889,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.68359375" customWidth="1"/>
-    <col min="9" max="9" width="35.68359375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="84.47265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.1015625" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="63.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="84.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2921,7 +2916,7 @@
         <v>45304.738252314812</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2929,7 +2924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2937,7 +2932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2945,12 +2940,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2958,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -2973,7 +2968,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
@@ -2985,13 +2980,13 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="M9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -3024,13 +3019,13 @@
         <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3060,13 +3055,13 @@
         <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="M11" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3</v>
       </c>
@@ -3096,13 +3091,13 @@
         <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M12" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -3113,10 +3108,10 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>280</v>
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
@@ -3126,22 +3121,22 @@
         <v>0.1</v>
       </c>
       <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
         <v>35</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -3149,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G14" s="1">
         <v>2.78</v>
@@ -3162,22 +3157,22 @@
         <v>2.78</v>
       </c>
       <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>40</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="L14" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H15" s="1">
         <f>SUM(H10:H14)</f>
         <v>21.300000000000004</v>

</xml_diff>

<commit_message>
clean up pico iCE traces
</commit_message>
<xml_diff>
--- a/BOM-nixieAccurateClock.xlsx
+++ b/BOM-nixieAccurateClock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Nextcloud\Documents\Projects\nixieclock\nixie-clock-ice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA6176E-D5BF-432E-9819-DA187A99C34E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB6C9D5-8ECB-499D-A34F-C170D810D006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="25644" windowHeight="15588" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nixie Accurate Clock" sheetId="5" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>BSP88</t>
   </si>
   <si>
-    <t>R1, R2, R10, R13</t>
-  </si>
-  <si>
     <t>4.7k</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>10M</t>
   </si>
   <si>
-    <t>R14, R15</t>
-  </si>
-  <si>
     <t>1k</t>
   </si>
   <si>
@@ -382,12 +376,6 @@
     <t>Device:C_Polarized</t>
   </si>
   <si>
-    <t>Capacitor_THT:CP_Radial_D10.0mm_P5.00mm</t>
-  </si>
-  <si>
-    <t>https://www.nichicon.co.jp/english/products/pdfs/e-uvc.pdf</t>
-  </si>
-  <si>
     <t>https://connect.kemet.com:7667/gateway/IntelliData-ComponentDocumentation/1.0/download/datasheet/C0603C102K5RACTU</t>
   </si>
   <si>
@@ -469,12 +457,6 @@
     <t>Switch:SW_DIP_x08</t>
   </si>
   <si>
-    <t>Button_Switch_THT:SW_DIP_SPSTx08_Slide_6.7x21.88mm_W7.62mm_P2.54mm_LowProfile</t>
-  </si>
-  <si>
-    <t>https://www.te.com/commerce/DocumentDelivery/DDEController?Action=srchrtrv&amp;DocNm=ADE_ADP_ADF_Datasheet&amp;DocType=Data+Sheet&amp;DocLang=English&amp;DocFormat=pdf&amp;PartCntxt=1825057-7</t>
-  </si>
-  <si>
     <t>Connector:TestPoint</t>
   </si>
   <si>
@@ -544,9 +526,6 @@
     <t>CL10A105KA8NNNC</t>
   </si>
   <si>
-    <t>UVC2G100MPD1TD</t>
-  </si>
-  <si>
     <t>C0603C102K5RAC7867</t>
   </si>
   <si>
@@ -604,9 +583,6 @@
     <t>3266Z-1-104LF</t>
   </si>
   <si>
-    <t>1825057-7</t>
-  </si>
-  <si>
     <t>ADC0820BCWMX/NOPB</t>
   </si>
   <si>
@@ -658,12 +634,6 @@
     <t>https://www.mouser.com/ProductDetail/Samsung-Electro-Mechanics/CL10A105KA8NNNC?qs=hqM3L16%252BxldY%252BnK4KzDJVg%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.com/ProductDetail/Nichicon/UVC2G100MPD1TD?qs=dHDuPHwQO7%2FySlLjjH7nrA%3D%3D</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/nichicon/UVC2G100MPD1TD/4312415</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/kemet/C0603C102K5RAC7867/411081</t>
   </si>
   <si>
@@ -805,12 +775,6 @@
     <t>https://www.mouser.com/ProductDetail/Bourns/3266Z-1-104LF?qs=%252B8v4bwhISUIlrQ43joPBoQ%3D%3D</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/te-connectivity-alcoswitch-switches/1825057-7/969176</t>
-  </si>
-  <si>
-    <t>https://www.mouser.com/ProductDetail/TE-Connectivity-PB/ADE0804?qs=k5V78Jg%2Feq6GvBeNB1YtWA%3D%3D</t>
-  </si>
-  <si>
     <t>https://www.mouser.com/ProductDetail/Microchip-Technology/MCP23008-E-SO?qs=Sez7gRs8XSWum74ZwQXTLw%3D%3D</t>
   </si>
   <si>
@@ -875,6 +839,42 @@
   </si>
   <si>
     <t>RC1206JR-0727KL</t>
+  </si>
+  <si>
+    <t>ULR2E100MNL1GS</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:CP_Elec_8x10</t>
+  </si>
+  <si>
+    <t>https://www.nichicon.co.jp/english/series_items/catalog_pdf/e-ulr.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/nichicon/ULR2E100MNL1GS/3664123</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Nichicon/ULR2E100MNL1GS?qs=aoAypCcaRa8pBYU9738QBQ%3D%3D</t>
+  </si>
+  <si>
+    <t>219-8MST</t>
+  </si>
+  <si>
+    <t>Button_Switch_SMD:SW_DIP_SPSTx08_Slide_6.7x21.88mm_W8.61mm_P2.54mm_LowProfile</t>
+  </si>
+  <si>
+    <t>https://www.ctscorp.com/wp-content/uploads/219.pdf</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/cts-electrocomponents/219-8MST/223209</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/CTS-Electronic-Components/219-8MST?qs=qNzHFtQhdJ%252B8jOs%2FDCRqeg%3D%3D</t>
+  </si>
+  <si>
+    <t>R10, R13</t>
+  </si>
+  <si>
+    <t>R1, R2, R14, R15</t>
   </si>
 </sst>
 </file>
@@ -946,9 +946,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -986,7 +986,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1092,7 +1092,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1234,7 +1234,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1339,10 +1339,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="M9" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1369,19 +1369,19 @@
         <v>1.22</v>
       </c>
       <c r="I10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J10" t="s">
-        <v>110</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1392,7 +1392,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1408,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="J11" t="s">
         <v>20</v>
@@ -1417,10 +1417,10 @@
         <v>21</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1447,19 +1447,19 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="I12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J12" t="s">
         <v>20</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1476,29 +1476,29 @@
         <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="G13" s="1">
-        <v>1.03</v>
+        <v>0.99</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="0"/>
-        <v>2.06</v>
+        <v>1.98</v>
       </c>
       <c r="I13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J13" t="s">
-        <v>116</v>
+        <v>270</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>117</v>
+        <v>271</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>209</v>
+        <v>272</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>208</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -1515,7 +1515,7 @@
         <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -1525,19 +1525,19 @@
         <v>0.1</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J14" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -1561,19 +1561,19 @@
         <v>0.81</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J15" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -1584,13 +1584,13 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D16" t="s">
         <v>55</v>
       </c>
       <c r="E16" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -1600,19 +1600,19 @@
         <v>0.70000000000000007</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="J16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1639,19 +1639,19 @@
         <v>7.55</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>59</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G18" s="1">
         <v>0.81</v>
@@ -1681,16 +1681,16 @@
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="M18" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1707,7 +1707,7 @@
         <v>61</v>
       </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G19" s="1">
         <v>0.38</v>
@@ -1717,19 +1717,19 @@
         <v>0.38</v>
       </c>
       <c r="I19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="J19" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
         <v>63</v>
       </c>
       <c r="E20" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="G20" s="1">
         <v>4.07</v>
@@ -1756,19 +1756,19 @@
         <v>4.07</v>
       </c>
       <c r="I20" t="s">
+        <v>126</v>
+      </c>
+      <c r="J20" t="s">
+        <v>129</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="J20" t="s">
-        <v>133</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="L20" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -1795,19 +1795,19 @@
         <v>2.75</v>
       </c>
       <c r="I21" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J21" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -1815,38 +1815,38 @@
         <v>13</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
+        <v>279</v>
+      </c>
+      <c r="D22" t="s">
         <v>66</v>
       </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
       <c r="E22" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="0"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="I22" t="s">
         <v>34</v>
       </c>
       <c r="J22" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K22" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -1857,13 +1857,13 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
         <v>68</v>
       </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -1876,16 +1876,16 @@
         <v>34</v>
       </c>
       <c r="J23" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -1896,13 +1896,13 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" t="s">
         <v>70</v>
       </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
       <c r="E24" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="G24" s="1">
         <v>0.1</v>
@@ -1915,16 +1915,16 @@
         <v>34</v>
       </c>
       <c r="J24" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -1935,13 +1935,13 @@
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
         <v>72</v>
       </c>
-      <c r="D25" t="s">
-        <v>73</v>
-      </c>
       <c r="E25" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="G25" s="1">
         <v>0.74</v>
@@ -1954,16 +1954,16 @@
         <v>34</v>
       </c>
       <c r="J25" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -1974,13 +1974,13 @@
         <v>10</v>
       </c>
       <c r="C26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
         <v>74</v>
       </c>
-      <c r="D26" t="s">
-        <v>75</v>
-      </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="G26" s="1">
         <v>0.1</v>
@@ -1993,16 +1993,16 @@
         <v>34</v>
       </c>
       <c r="J26" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -2013,13 +2013,13 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27">
         <v>470</v>
       </c>
       <c r="E27" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="G27" s="1">
         <v>0.1</v>
@@ -2032,16 +2032,16 @@
         <v>34</v>
       </c>
       <c r="J27" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -2052,13 +2052,13 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
         <v>77</v>
       </c>
-      <c r="D28" t="s">
-        <v>78</v>
-      </c>
       <c r="E28" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="G28" s="1">
         <v>0.1</v>
@@ -2071,16 +2071,16 @@
         <v>34</v>
       </c>
       <c r="J28" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
@@ -2088,38 +2088,38 @@
         <v>20</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>79</v>
+        <v>280</v>
       </c>
       <c r="D29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G29" s="1">
         <v>0.1</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I29" t="s">
         <v>34</v>
       </c>
       <c r="J29" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -2130,13 +2130,13 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="G30" s="1">
         <v>0.1</v>
@@ -2149,16 +2149,16 @@
         <v>34</v>
       </c>
       <c r="J30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -2169,13 +2169,13 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="G31" s="1">
         <v>0.1</v>
@@ -2188,16 +2188,16 @@
         <v>34</v>
       </c>
       <c r="J31" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K31" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -2208,13 +2208,13 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="G32" s="1">
         <v>0.1</v>
@@ -2227,16 +2227,16 @@
         <v>34</v>
       </c>
       <c r="J32" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K32" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -2247,13 +2247,13 @@
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E33" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G33" s="1">
         <v>0.1</v>
@@ -2266,16 +2266,16 @@
         <v>34</v>
       </c>
       <c r="J33" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>36</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -2286,13 +2286,13 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="G34" s="1">
         <v>0.1</v>
@@ -2305,16 +2305,16 @@
         <v>34</v>
       </c>
       <c r="J34" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -2325,13 +2325,13 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G35" s="1">
         <v>0.43</v>
@@ -2344,16 +2344,16 @@
         <v>34</v>
       </c>
       <c r="J35" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -2364,13 +2364,13 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="G36" s="1">
         <v>2.13</v>
@@ -2380,19 +2380,19 @@
         <v>2.13</v>
       </c>
       <c r="I36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -2403,35 +2403,35 @@
         <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E37" t="s">
-        <v>190</v>
+        <v>274</v>
       </c>
       <c r="G37" s="1">
-        <v>1.75</v>
+        <v>0.95</v>
       </c>
       <c r="H37" s="1">
         <f t="shared" si="0"/>
-        <v>1.75</v>
+        <v>0.95</v>
       </c>
       <c r="I37" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="J37" t="s">
-        <v>145</v>
+        <v>275</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>146</v>
+        <v>276</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>258</v>
+        <v>278</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -2442,10 +2442,10 @@
         <v>20</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E38">
         <v>5019</v>
@@ -2458,19 +2458,19 @@
         <v>6.6000000000000005</v>
       </c>
       <c r="I38" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="J38" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="K38" s="3" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -2484,10 +2484,10 @@
         <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E39" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="G39" s="1">
         <v>1.37</v>
@@ -2497,19 +2497,19 @@
         <v>1.37</v>
       </c>
       <c r="I39" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="J39" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
@@ -2520,10 +2520,10 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G40" s="1">
         <v>35</v>
@@ -2533,19 +2533,19 @@
         <v>35</v>
       </c>
       <c r="I40" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="J40" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="L40" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M40" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
@@ -2556,10 +2556,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G41" s="1">
         <v>0.97</v>
@@ -2569,19 +2569,19 @@
         <v>0.97</v>
       </c>
       <c r="I41" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="J41" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
@@ -2592,10 +2592,10 @@
         <v>1</v>
       </c>
       <c r="C42" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G42" s="1">
         <v>27.8</v>
@@ -2605,19 +2605,19 @@
         <v>27.8</v>
       </c>
       <c r="I42" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="J42" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="L42" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M42" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
@@ -2628,13 +2628,13 @@
         <v>2</v>
       </c>
       <c r="C43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G43" s="1">
         <v>2.1800000000000002</v>
@@ -2644,19 +2644,19 @@
         <v>4.3600000000000003</v>
       </c>
       <c r="I43" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J43" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
@@ -2667,7 +2667,7 @@
         <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G44" s="1">
         <f>'IN-14 daughter board'!H15</f>
@@ -2678,16 +2678,16 @@
         <v>127.80000000000003</v>
       </c>
       <c r="I44" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="J44" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="L44" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M44" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
@@ -2698,13 +2698,13 @@
         <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E45" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G45" s="1">
         <v>5.93</v>
@@ -2714,19 +2714,19 @@
         <v>5.93</v>
       </c>
       <c r="I45" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="J45" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="K45" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
@@ -2737,13 +2737,13 @@
         <v>2</v>
       </c>
       <c r="C46" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D46" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E46" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G46" s="1">
         <v>1.65</v>
@@ -2753,25 +2753,25 @@
         <v>3.3</v>
       </c>
       <c r="I46" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="J46" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="K46" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H47" s="1">
         <f>SUM(H10:H46)</f>
-        <v>243.97000000000003</v>
+        <v>243.09000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2980,10 +2980,10 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="M9" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3019,10 +3019,10 @@
         <v>21</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -3055,10 +3055,10 @@
         <v>26</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="M11" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -3091,10 +3091,10 @@
         <v>32</v>
       </c>
       <c r="L12" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="M12" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -3108,10 +3108,10 @@
         <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
@@ -3130,10 +3130,10 @@
         <v>36</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -3166,10 +3166,10 @@
         <v>41</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>